<commit_message>
comboBox for origin destination
</commit_message>
<xml_diff>
--- a/gabari.xlsx
+++ b/gabari.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="لرستان" sheetId="1" r:id="rId1"/>
@@ -1391,7 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView rightToLeft="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
@@ -2439,7 +2439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView rightToLeft="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>

</xml_diff>